<commit_message>
Changes v2 25 02
</commit_message>
<xml_diff>
--- a/pK-EP-v.1.0.2/Excel Files/crank_slide_2D_Nikra.xlsx
+++ b/pK-EP-v.1.0.2/Excel Files/crank_slide_2D_Nikra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\pK-EP-v.1.0.2\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D212AE-16C4-46CA-95D2-E08F41A6D822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153AF405-3279-41C9-8840-84F192A582BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,24 +561,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,7 +576,25 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -615,10 +615,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1023,18 +1023,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="13">
         <v>0</v>
       </c>
@@ -1044,10 +1044,10 @@
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="13">
         <v>0</v>
       </c>
@@ -1057,10 +1057,10 @@
       <c r="S5" s="16"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="13">
         <v>0</v>
       </c>
@@ -1070,10 +1070,10 @@
       <c r="S6" s="16"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="41"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="13">
         <v>0</v>
       </c>
@@ -1089,18 +1089,18 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="17">
         <v>2</v>
       </c>
@@ -1109,10 +1109,10 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="17">
         <v>0.5</v>
       </c>
@@ -1127,58 +1127,58 @@
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="40"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="35"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="34"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="34"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="41"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
         <v>41</v>
@@ -1186,11 +1186,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B11:C11"/>
@@ -1200,6 +1195,11 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4746,8 +4746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4806,11 +4806,11 @@
       <c r="E2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4948,21 +4948,21 @@
       <c r="E7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50" t="s">
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50" t="s">
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -5000,19 +5000,19 @@
         <v>663</v>
       </c>
       <c r="J8" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="27">
         <v>663</v>
       </c>
       <c r="M8" s="27">
+        <v>0</v>
+      </c>
+      <c r="N8" s="27">
         <v>1</v>
-      </c>
-      <c r="N8" s="27">
-        <v>0</v>
       </c>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
@@ -5081,16 +5081,16 @@
       <c r="E11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="50" t="s">
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5205,16 +5205,16 @@
       <c r="E16" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="50" t="s">
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25">
@@ -5310,16 +5310,16 @@
       <c r="E20" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="49" t="s">
+      <c r="F20" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50" t="s">
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
     </row>
     <row r="21" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -5509,11 +5509,11 @@
       <c r="H31" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="50" t="s">
+      <c r="I31" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
     </row>
     <row r="32" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
@@ -5587,11 +5587,11 @@
       <c r="D35" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="50" t="s">
+      <c r="E35" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
@@ -5697,6 +5697,18 @@
     <row r="52" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="A19:K19"/>
@@ -5706,18 +5718,6 @@
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A30:K30"/>
     <mergeCell ref="I31:K31"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B29 B18 B32:B33" xr:uid="{00000000-0002-0000-0100-000001000000}">

</xml_diff>

<commit_message>
Changes previous day 09 03
</commit_message>
<xml_diff>
--- a/pK-EP-v.1.0.2/Excel Files/crank_slide_2D_Nikra.xlsx
+++ b/pK-EP-v.1.0.2/Excel Files/crank_slide_2D_Nikra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\pK-EP-v.1.0.2\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BEB94D-360D-4370-BCBC-783A7DA6A8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EB27CF-6711-4408-8879-B1A3D1C62CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Motions" sheetId="4" r:id="rId1"/>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B3:S18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I7:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4746,8 +4746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:K17"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O26" sqref="O25:O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes 09 03 Afternoon
</commit_message>
<xml_diff>
--- a/pK-EP-v.1.0.2/Excel Files/crank_slide_2D_Nikra.xlsx
+++ b/pK-EP-v.1.0.2/Excel Files/crank_slide_2D_Nikra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\pK-EP-v.1.0.2\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EB27CF-6711-4408-8879-B1A3D1C62CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009B8C8F-57FE-4BF0-B622-490F6E2C48A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,6 +561,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,25 +594,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -615,10 +615,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1012,7 +1012,7 @@
   <dimension ref="B3:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I7:I8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,18 +1023,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="13">
         <v>0</v>
       </c>
@@ -1044,10 +1044,10 @@
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="13">
         <v>0</v>
       </c>
@@ -1057,10 +1057,10 @@
       <c r="S5" s="16"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="13">
         <v>0</v>
       </c>
@@ -1070,10 +1070,10 @@
       <c r="S6" s="16"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="35"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="13">
         <v>0</v>
       </c>
@@ -1089,18 +1089,18 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="17">
         <v>2</v>
       </c>
@@ -1109,10 +1109,10 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="17">
         <v>0.5</v>
       </c>
@@ -1127,58 +1127,58 @@
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="41"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="41"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="41"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="41"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
         <v>41</v>
@@ -1186,6 +1186,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B11:C11"/>
@@ -1195,11 +1200,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4746,8 +4746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O26" sqref="O25:O26"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4806,11 +4806,11 @@
       <c r="E2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4948,21 +4948,21 @@
       <c r="E7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="49" t="s">
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49" t="s">
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -5081,16 +5081,16 @@
       <c r="E11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="49" t="s">
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5205,16 +5205,16 @@
       <c r="E16" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="50" t="s">
+      <c r="F16" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="49" t="s">
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
@@ -5288,16 +5288,16 @@
       <c r="E20" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="49" t="s">
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
     </row>
     <row r="21" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
@@ -5521,11 +5521,11 @@
       <c r="H31" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="49" t="s">
+      <c r="I31" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
     </row>
     <row r="32" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
@@ -5599,11 +5599,11 @@
       <c r="D35" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="49" t="s">
+      <c r="E35" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
@@ -5709,18 +5709,6 @@
     <row r="52" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="A19:K19"/>
@@ -5730,6 +5718,18 @@
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A30:K30"/>
     <mergeCell ref="I31:K31"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B29 B18 B32:B33" xr:uid="{00000000-0002-0000-0100-000001000000}">

</xml_diff>

<commit_message>
Changes 11 03 morning
</commit_message>
<xml_diff>
--- a/pK-EP-v.1.0.2/Excel Files/crank_slide_2D_Nikra.xlsx
+++ b/pK-EP-v.1.0.2/Excel Files/crank_slide_2D_Nikra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\pK-EP-v.1.0.2\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009B8C8F-57FE-4BF0-B622-490F6E2C48A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6EF5A6-8E46-4904-A1B3-FAB41B39F861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Motions" sheetId="4" r:id="rId1"/>
@@ -276,7 +276,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -330,14 +330,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -489,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -522,9 +514,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -546,7 +535,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -555,28 +544,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -594,7 +565,25 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -615,10 +604,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1011,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B3:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,18 +1012,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="13">
         <v>0</v>
       </c>
@@ -1044,10 +1033,10 @@
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="13">
         <v>0</v>
       </c>
@@ -1057,10 +1046,10 @@
       <c r="S5" s="16"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="13">
         <v>0</v>
       </c>
@@ -1070,10 +1059,10 @@
       <c r="S6" s="16"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="41"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="13">
         <v>0</v>
       </c>
@@ -1089,18 +1078,18 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="17">
         <v>2</v>
       </c>
@@ -1109,10 +1098,10 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="17">
         <v>0.5</v>
       </c>
@@ -1127,12 +1116,12 @@
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="35" t="s">
@@ -1145,40 +1134,40 @@
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="34"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="34"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
         <v>41</v>
@@ -1186,11 +1175,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B11:C11"/>
@@ -1200,6 +1184,11 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1211,7 +1200,7 @@
   <dimension ref="A1:AB197"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:G16"/>
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,435 +1218,432 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="43"/>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44" t="s">
+      <c r="A1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44" t="s">
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44" t="s">
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="46" t="s">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46" t="s">
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46" t="s">
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="44" t="s">
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44" t="s">
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="47" t="s">
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="S2" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="46" t="s">
+      <c r="S2" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="O3" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="P3" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="Q3" s="22" t="s">
+      <c r="Q3" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="47"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="22" t="s">
+      <c r="R3" s="46"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="22" t="s">
+      <c r="U3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="22" t="s">
+      <c r="V3" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="21">
         <v>1</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="22">
-        <v>0</v>
-      </c>
-      <c r="D4" s="22">
-        <v>0</v>
-      </c>
-      <c r="E4" s="22">
-        <v>0</v>
-      </c>
-      <c r="F4" s="22">
-        <v>0</v>
-      </c>
-      <c r="G4" s="22">
-        <v>0</v>
-      </c>
-      <c r="H4" s="22">
-        <v>0</v>
-      </c>
-      <c r="I4" s="22">
-        <v>0</v>
-      </c>
-      <c r="J4" s="22">
-        <v>0</v>
-      </c>
-      <c r="K4" s="22">
-        <v>0</v>
-      </c>
-      <c r="L4" s="22">
-        <v>0</v>
-      </c>
-      <c r="M4" s="22">
-        <v>0</v>
-      </c>
-      <c r="N4" s="22">
-        <v>0</v>
-      </c>
-      <c r="O4" s="22">
-        <v>0</v>
-      </c>
-      <c r="P4" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="24">
-        <v>0</v>
-      </c>
-      <c r="R4" s="24">
-        <v>0</v>
-      </c>
-      <c r="S4" s="22">
-        <v>0</v>
-      </c>
-      <c r="T4" s="22">
-        <v>0</v>
-      </c>
-      <c r="U4" s="22">
-        <v>0</v>
-      </c>
-      <c r="V4" s="22">
+      <c r="C4" s="21">
+        <v>0</v>
+      </c>
+      <c r="D4" s="21">
+        <v>0</v>
+      </c>
+      <c r="E4" s="21">
+        <v>0</v>
+      </c>
+      <c r="F4" s="21">
+        <v>0</v>
+      </c>
+      <c r="G4" s="21">
+        <v>0</v>
+      </c>
+      <c r="H4" s="21">
+        <v>0</v>
+      </c>
+      <c r="I4" s="21">
+        <v>0</v>
+      </c>
+      <c r="J4" s="21">
+        <v>0</v>
+      </c>
+      <c r="K4" s="21">
+        <v>0</v>
+      </c>
+      <c r="L4" s="21">
+        <v>0</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0</v>
+      </c>
+      <c r="N4" s="21">
+        <v>0</v>
+      </c>
+      <c r="O4" s="21">
+        <v>0</v>
+      </c>
+      <c r="P4" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>0</v>
+      </c>
+      <c r="R4" s="23">
+        <v>0</v>
+      </c>
+      <c r="S4" s="21">
+        <v>0</v>
+      </c>
+      <c r="T4" s="21">
+        <v>0</v>
+      </c>
+      <c r="U4" s="21">
+        <v>0</v>
+      </c>
+      <c r="V4" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>2</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="22">
         <v>86.6</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>50</v>
       </c>
-      <c r="E5" s="30">
-        <v>0</v>
-      </c>
-      <c r="F5" s="22">
-        <v>0</v>
-      </c>
-      <c r="G5" s="22">
-        <v>0</v>
-      </c>
-      <c r="H5" s="22">
-        <v>0</v>
-      </c>
-      <c r="I5" s="22">
-        <v>0</v>
-      </c>
-      <c r="J5" s="22">
-        <v>0</v>
-      </c>
-      <c r="K5" s="22">
-        <v>0</v>
-      </c>
-      <c r="L5" s="22">
-        <v>0</v>
-      </c>
-      <c r="M5" s="22">
-        <v>0</v>
-      </c>
-      <c r="N5" s="22">
-        <v>0</v>
-      </c>
-      <c r="O5" s="22">
-        <v>0</v>
-      </c>
-      <c r="P5" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="24">
+      <c r="E5" s="29">
+        <v>0</v>
+      </c>
+      <c r="F5" s="21">
+        <v>0</v>
+      </c>
+      <c r="G5" s="21">
+        <v>0</v>
+      </c>
+      <c r="H5" s="21">
+        <v>0</v>
+      </c>
+      <c r="I5" s="21">
+        <v>0</v>
+      </c>
+      <c r="J5" s="21">
+        <v>0</v>
+      </c>
+      <c r="K5" s="21">
+        <v>0</v>
+      </c>
+      <c r="L5" s="21">
+        <v>0</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0</v>
+      </c>
+      <c r="N5" s="21">
+        <v>0</v>
+      </c>
+      <c r="O5" s="21">
+        <v>0</v>
+      </c>
+      <c r="P5" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="23">
         <v>1</v>
       </c>
-      <c r="R5" s="24">
+      <c r="R5" s="23">
         <v>0.52359999999999995</v>
       </c>
-      <c r="S5" s="22">
-        <v>0</v>
-      </c>
-      <c r="T5" s="22">
-        <v>0</v>
-      </c>
-      <c r="U5" s="22">
-        <v>0</v>
-      </c>
-      <c r="V5" s="22">
+      <c r="S5" s="21">
+        <v>0</v>
+      </c>
+      <c r="T5" s="21">
+        <v>0</v>
+      </c>
+      <c r="U5" s="21">
+        <v>0</v>
+      </c>
+      <c r="V5" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>3</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="22">
         <v>467.13</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <v>40</v>
       </c>
-      <c r="E6" s="30">
-        <v>0</v>
-      </c>
-      <c r="F6" s="22">
-        <v>0</v>
-      </c>
-      <c r="G6" s="22">
-        <v>0</v>
-      </c>
-      <c r="H6" s="22">
-        <v>0</v>
-      </c>
-      <c r="I6" s="22">
-        <v>0</v>
-      </c>
-      <c r="J6" s="22">
-        <v>0</v>
-      </c>
-      <c r="K6" s="22">
-        <v>0</v>
-      </c>
-      <c r="L6" s="24">
-        <v>0</v>
-      </c>
-      <c r="M6" s="24">
-        <v>0</v>
-      </c>
-      <c r="N6" s="24">
-        <v>0</v>
-      </c>
-      <c r="O6" s="24">
-        <v>0</v>
-      </c>
-      <c r="P6" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="24">
+      <c r="E6" s="29">
+        <v>0</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0</v>
+      </c>
+      <c r="I6" s="21">
+        <v>0</v>
+      </c>
+      <c r="J6" s="21">
+        <v>0</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0</v>
+      </c>
+      <c r="L6" s="23">
+        <v>0</v>
+      </c>
+      <c r="M6" s="23">
+        <v>0</v>
+      </c>
+      <c r="N6" s="23">
+        <v>0</v>
+      </c>
+      <c r="O6" s="23">
+        <v>0</v>
+      </c>
+      <c r="P6" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="23">
         <v>1</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="23">
         <v>-0.20100000000000001</v>
       </c>
-      <c r="S6" s="22">
-        <v>0</v>
-      </c>
-      <c r="T6" s="22">
-        <v>0</v>
-      </c>
-      <c r="U6" s="22">
-        <v>0</v>
-      </c>
-      <c r="V6" s="22">
+      <c r="S6" s="21">
+        <v>0</v>
+      </c>
+      <c r="T6" s="21">
+        <v>0</v>
+      </c>
+      <c r="U6" s="21">
+        <v>0</v>
+      </c>
+      <c r="V6" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>4</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="21">
         <v>700</v>
       </c>
-      <c r="D7" s="22">
-        <v>0</v>
-      </c>
-      <c r="E7" s="22">
-        <v>0</v>
-      </c>
-      <c r="F7" s="22">
-        <v>0</v>
-      </c>
-      <c r="G7" s="22">
-        <v>0</v>
-      </c>
-      <c r="H7" s="22">
-        <v>0</v>
-      </c>
-      <c r="I7" s="22">
-        <v>0</v>
-      </c>
-      <c r="J7" s="22">
-        <v>0</v>
-      </c>
-      <c r="K7" s="22">
-        <v>0</v>
-      </c>
-      <c r="L7" s="22">
-        <v>0</v>
-      </c>
-      <c r="M7" s="22">
-        <v>0</v>
-      </c>
-      <c r="N7" s="22">
-        <v>0</v>
-      </c>
-      <c r="O7" s="22">
-        <v>0</v>
-      </c>
-      <c r="P7" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="24">
-        <v>0</v>
-      </c>
-      <c r="R7" s="24">
-        <v>0</v>
-      </c>
-      <c r="S7" s="22">
-        <v>0</v>
-      </c>
-      <c r="T7" s="22">
-        <v>0</v>
-      </c>
-      <c r="U7" s="22">
-        <v>0</v>
-      </c>
-      <c r="V7" s="22">
+      <c r="D7" s="21">
+        <v>0</v>
+      </c>
+      <c r="E7" s="21">
+        <v>0</v>
+      </c>
+      <c r="F7" s="21">
+        <v>0</v>
+      </c>
+      <c r="G7" s="21">
+        <v>0</v>
+      </c>
+      <c r="H7" s="21">
+        <v>0</v>
+      </c>
+      <c r="I7" s="21">
+        <v>0</v>
+      </c>
+      <c r="J7" s="21">
+        <v>0</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0</v>
+      </c>
+      <c r="L7" s="21">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0</v>
+      </c>
+      <c r="N7" s="21">
+        <v>0</v>
+      </c>
+      <c r="O7" s="21">
+        <v>0</v>
+      </c>
+      <c r="P7" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="23">
+        <v>0</v>
+      </c>
+      <c r="R7" s="23">
+        <v>0</v>
+      </c>
+      <c r="S7" s="21">
+        <v>0</v>
+      </c>
+      <c r="T7" s="21">
+        <v>0</v>
+      </c>
+      <c r="U7" s="21">
+        <v>0</v>
+      </c>
+      <c r="V7" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="18"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -1665,12 +1651,12 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1887,7 +1873,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="19"/>
+      <c r="O21" s="18"/>
       <c r="P21" s="3"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
@@ -1905,7 +1891,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="19"/>
+      <c r="O22" s="18"/>
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
@@ -1923,7 +1909,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="19"/>
+      <c r="O23" s="18"/>
       <c r="P23" s="3"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
@@ -1941,7 +1927,7 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="19"/>
+      <c r="O24" s="18"/>
       <c r="P24" s="3"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
@@ -1959,7 +1945,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="19"/>
+      <c r="O25" s="18"/>
       <c r="P25" s="3"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
@@ -1977,7 +1963,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="19"/>
+      <c r="O26" s="18"/>
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
@@ -1995,7 +1981,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="19"/>
+      <c r="O27" s="18"/>
       <c r="P27" s="3"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
@@ -2013,7 +1999,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="19"/>
+      <c r="O28" s="18"/>
       <c r="P28" s="3"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
@@ -4744,10 +4730,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X52"/>
+  <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:F23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4766,16 +4752,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -4791,19 +4777,19 @@
       <c r="X1" s="10"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="49" t="s">
@@ -4850,9 +4836,9 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
@@ -4862,20 +4848,20 @@
       <c r="X3" s="10"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
@@ -4885,14 +4871,14 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -4908,22 +4894,22 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
@@ -4953,16 +4939,16 @@
       </c>
       <c r="G7" s="49"/>
       <c r="H7" s="49"/>
-      <c r="I7" s="50" t="s">
+      <c r="I7" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50" t="s">
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -4972,46 +4958,46 @@
       <c r="X7" s="10"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="24">
         <v>4</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="18">
         <v>3</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="18">
         <v>4</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="18">
         <v>663</v>
       </c>
-      <c r="G8" s="19">
-        <v>0</v>
-      </c>
-      <c r="H8" s="19">
-        <v>0</v>
-      </c>
-      <c r="I8" s="25">
+      <c r="G8" s="18">
+        <v>0</v>
+      </c>
+      <c r="H8" s="18">
+        <v>0</v>
+      </c>
+      <c r="I8" s="24">
         <v>663</v>
       </c>
-      <c r="J8" s="25">
-        <v>0</v>
-      </c>
-      <c r="K8" s="25">
+      <c r="J8" s="24">
+        <v>0</v>
+      </c>
+      <c r="K8" s="24">
         <v>1</v>
       </c>
-      <c r="L8" s="27">
+      <c r="L8" s="26">
         <v>663</v>
       </c>
-      <c r="M8" s="27">
+      <c r="M8" s="26">
         <v>1</v>
       </c>
-      <c r="N8" s="27">
+      <c r="N8" s="26">
         <v>0</v>
       </c>
       <c r="R8" s="10"/>
@@ -5044,19 +5030,19 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5066,7 +5052,7 @@
       <c r="X10" s="10"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -5086,11 +5072,11 @@
       </c>
       <c r="G11" s="49"/>
       <c r="H11" s="49"/>
-      <c r="I11" s="50" t="s">
+      <c r="I11" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5100,37 +5086,37 @@
       <c r="X11" s="10"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="18">
         <v>2</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>1</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="18">
         <v>2</v>
       </c>
-      <c r="F12" s="19">
-        <v>0</v>
-      </c>
-      <c r="G12" s="19">
-        <v>0</v>
-      </c>
-      <c r="H12" s="19">
-        <v>0</v>
-      </c>
-      <c r="I12" s="19">
-        <v>0</v>
-      </c>
-      <c r="J12" s="19">
-        <v>0</v>
-      </c>
-      <c r="K12" s="19">
+      <c r="F12" s="18">
+        <v>0</v>
+      </c>
+      <c r="G12" s="18">
+        <v>0</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0</v>
+      </c>
+      <c r="I12" s="18">
+        <v>0</v>
+      </c>
+      <c r="J12" s="18">
+        <v>0</v>
+      </c>
+      <c r="K12" s="18">
         <v>1</v>
       </c>
       <c r="R12" s="10"/>
@@ -5141,24 +5127,24 @@
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
+    <row r="13" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
@@ -5168,19 +5154,19 @@
       <c r="X14" s="10"/>
     </row>
     <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
@@ -5190,19 +5176,19 @@
       <c r="X15" s="10"/>
     </row>
     <row r="16" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="20" t="s">
         <v>16</v>
       </c>
       <c r="F16" s="49" t="s">
@@ -5210,24 +5196,24 @@
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
-      <c r="I16" s="50" t="s">
+      <c r="I16" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
     </row>
     <row r="18" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
@@ -5251,19 +5237,19 @@
       <c r="X18" s="10"/>
     </row>
     <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -5273,19 +5259,19 @@
       <c r="X19" s="10"/>
     </row>
     <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="20" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="49" t="s">
@@ -5293,57 +5279,57 @@
       </c>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
-      <c r="I20" s="50" t="s">
+      <c r="I20" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-    </row>
-    <row r="21" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25">
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+    </row>
+    <row r="21" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
         <v>5</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="24">
         <v>4</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="24">
         <v>1</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="24">
         <v>763</v>
       </c>
-      <c r="G21" s="25">
-        <v>0</v>
-      </c>
-      <c r="H21" s="25">
-        <v>0</v>
-      </c>
-      <c r="I21" s="25">
+      <c r="G21" s="24">
+        <v>0</v>
+      </c>
+      <c r="H21" s="24">
+        <v>0</v>
+      </c>
+      <c r="I21" s="24">
         <v>1</v>
       </c>
-      <c r="J21" s="25">
-        <v>0</v>
-      </c>
-      <c r="K21" s="25">
+      <c r="J21" s="24">
+        <v>0</v>
+      </c>
+      <c r="K21" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
@@ -5358,22 +5344,22 @@
       <c r="X23" s="10"/>
     </row>
     <row r="24" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="20" t="s">
         <v>25</v>
       </c>
       <c r="G24" s="12"/>
@@ -5404,12 +5390,12 @@
       <c r="X25" s="10"/>
     </row>
     <row r="26" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
@@ -5426,7 +5412,7 @@
       <c r="X26" s="10"/>
     </row>
     <row r="27" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -5468,275 +5454,288 @@
       <c r="K28" s="11"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="9"/>
-    </row>
-    <row r="30" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="51" t="s">
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="9"/>
+    </row>
+    <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
-    </row>
-    <row r="31" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="51"/>
+    </row>
+    <row r="32" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B32" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C32" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D32" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E32" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="F32" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="G31" s="21" t="s">
+      <c r="G32" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="H31" s="21" t="s">
+      <c r="H32" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="50" t="s">
+      <c r="I32" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-    </row>
-    <row r="32" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+    </row>
+    <row r="33" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
         <v>2</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B33" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C33" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D33" s="18">
         <v>2</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E33" s="18">
         <v>0.52300000000000002</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F33" s="18">
         <v>-0.3</v>
       </c>
-      <c r="G32" s="19">
-        <v>0</v>
-      </c>
-      <c r="H32" s="19">
+      <c r="G33" s="18">
+        <v>0</v>
+      </c>
+      <c r="H33" s="18">
         <v>6</v>
       </c>
-      <c r="I32" s="12">
-        <v>0</v>
-      </c>
-      <c r="J32" s="12">
-        <v>0</v>
-      </c>
-      <c r="K32" s="12">
+      <c r="I33" s="12">
+        <v>0</v>
+      </c>
+      <c r="J33" s="12">
+        <v>0</v>
+      </c>
+      <c r="K33" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-    </row>
-    <row r="34" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="48" t="s">
+    <row r="34" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+    </row>
+    <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
+      <c r="B35" s="47"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="50" t="s">
+      <c r="E36" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="19">
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="18">
         <v>1</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B37" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C37" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D37" s="18">
         <v>1</v>
       </c>
-      <c r="E36" s="19">
-        <v>0</v>
-      </c>
-      <c r="F36" s="19">
-        <v>0</v>
-      </c>
-      <c r="G36" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="19">
+      <c r="E37" s="18">
+        <v>0</v>
+      </c>
+      <c r="F37" s="18">
+        <v>0</v>
+      </c>
+      <c r="G37" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
         <v>2</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B38" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C38" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D38" s="18">
         <v>2</v>
       </c>
-      <c r="E37" s="19">
+      <c r="E38" s="18">
         <v>173.2</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F38" s="18">
         <v>100</v>
       </c>
-      <c r="G37" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="19">
+      <c r="G38" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="18">
         <v>3</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B39" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C39" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="19">
+      <c r="D39" s="18">
         <v>3</v>
       </c>
-      <c r="E38" s="19">
+      <c r="E39" s="18">
         <v>663</v>
       </c>
-      <c r="F38" s="19">
-        <v>0</v>
-      </c>
-      <c r="G38" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="19">
+      <c r="F39" s="18">
+        <v>0</v>
+      </c>
+      <c r="G39" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="18">
         <v>4</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B40" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C40" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="19">
+      <c r="D40" s="18">
         <v>4</v>
       </c>
-      <c r="E39" s="19">
+      <c r="E40" s="18">
         <v>763</v>
       </c>
-      <c r="F39" s="19">
-        <v>0</v>
-      </c>
-      <c r="G39" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-    </row>
-    <row r="52" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F40" s="18">
+        <v>0</v>
+      </c>
+      <c r="G40" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+    </row>
+    <row r="53" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A30:K30"/>
-    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
     <mergeCell ref="A10:K10"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="I32:K32"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B29 B18 B32:B33" xr:uid="{00000000-0002-0000-0100-000001000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30 B18 B33:B34" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Spherical,Universal,Revolute,Translation,Cylindrical,Simple,Ground,Driver"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:B1026" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37:B1027" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Spherical,Universal,Revolute,Cylindrical,Translation,Simple,Driver,Ground,Point"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>